<commit_message>
add mapping for BFO 1.1 process which is used as range of property 'is duration of'
</commit_message>
<xml_diff>
--- a/branches/2014-06-13/doc/termsMapping.xlsx
+++ b/branches/2014-06-13/doc/termsMapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
   <si>
     <t>http://purl.org/obo/owl/OBO_REL#bearer_of</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/iao/dev/iao-main.owl#componet_of_information_entity</t>
+  </si>
+  <si>
+    <t>http://www.ifomis.org/bfo/1.1/span#Process</t>
   </si>
 </sst>
 </file>
@@ -775,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,16 +1056,16 @@
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1070,16 +1073,16 @@
     </row>
     <row r="17" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1087,16 +1090,16 @@
     </row>
     <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1104,16 +1107,16 @@
     </row>
     <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>15</v>
+        <v>52</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>92</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1121,125 +1124,123 @@
     </row>
     <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>96</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>34</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>84</v>
-      </c>
+      <c r="D22" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>99</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>102</v>
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="D24" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>96</v>
@@ -1248,74 +1249,74 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>48</v>
+      <c r="A26" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>87</v>
+      <c r="D26" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>49</v>
+      <c r="A29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>94</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>86</v>
@@ -1323,56 +1324,75 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A50" r:id="rId1" location="function_of"/>
-    <hyperlink ref="A52" r:id="rId2" location="quality_of"/>
-    <hyperlink ref="A53" r:id="rId3" location="role_of"/>
-    <hyperlink ref="B50" r:id="rId4"/>
-    <hyperlink ref="B52" r:id="rId5"/>
-    <hyperlink ref="B53" r:id="rId6"/>
+    <hyperlink ref="A51" r:id="rId1" location="function_of"/>
+    <hyperlink ref="A53" r:id="rId2" location="quality_of"/>
+    <hyperlink ref="A54" r:id="rId3" location="role_of"/>
+    <hyperlink ref="B51" r:id="rId4"/>
+    <hyperlink ref="B53" r:id="rId5"/>
+    <hyperlink ref="B54" r:id="rId6"/>
     <hyperlink ref="A2" r:id="rId7" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%23Entity"/>
     <hyperlink ref="B2" r:id="rId8" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000001"/>
     <hyperlink ref="A3" r:id="rId9" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23Continuant"/>
@@ -1401,38 +1421,40 @@
     <hyperlink ref="B14" r:id="rId32" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000003"/>
     <hyperlink ref="A15" r:id="rId33" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fspan%23ProcessualEntity"/>
     <hyperlink ref="B15" r:id="rId34" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000015"/>
-    <hyperlink ref="A16" r:id="rId35" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23ZeroDimensionalRegion"/>
-    <hyperlink ref="B16" r:id="rId36" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000018"/>
-    <hyperlink ref="A17" r:id="rId37" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23OneDimensionalRegion"/>
-    <hyperlink ref="B17" r:id="rId38" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000026"/>
-    <hyperlink ref="A18" r:id="rId39" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23TwoDimensionalRegion"/>
-    <hyperlink ref="B18" r:id="rId40" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000009"/>
-    <hyperlink ref="A19" r:id="rId41" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23ThreeDimensionalRegion"/>
-    <hyperlink ref="B19" r:id="rId42" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000028"/>
-    <hyperlink ref="A20" r:id="rId43" display="//www.google.com/url?q=http%3A%2F%2Fpurl.org%2Fobo%2Fowl%2FOBO_REL%23bearer_of"/>
-    <hyperlink ref="B20" r:id="rId44" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000053"/>
-    <hyperlink ref="A21" r:id="rId45" display="//www.google.com/url?q=http%3A%2F%2Fpurl.org%2Fobo%2Fowl%2FOBO_REL%23inheres_in"/>
-    <hyperlink ref="B21" r:id="rId46" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000052"/>
-    <hyperlink ref="A22" r:id="rId47" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_part"/>
-    <hyperlink ref="G22" r:id="rId48" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000051"/>
-    <hyperlink ref="A23" r:id="rId49" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23part_of"/>
-    <hyperlink ref="G23" r:id="rId50" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000050"/>
-    <hyperlink ref="A24" r:id="rId51" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_participant"/>
-    <hyperlink ref="B24" r:id="rId52" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000057"/>
-    <hyperlink ref="A25" r:id="rId53" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23participates_in"/>
-    <hyperlink ref="B25" r:id="rId54" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000056"/>
-    <hyperlink ref="A26" r:id="rId55" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000294"/>
-    <hyperlink ref="B26" r:id="rId56" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000059"/>
-    <hyperlink ref="A27" r:id="rId57" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000297"/>
-    <hyperlink ref="B27" r:id="rId58" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000058"/>
-    <hyperlink ref="A28" r:id="rId59" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000300"/>
-    <hyperlink ref="B28" r:id="rId60" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000054"/>
-    <hyperlink ref="A29" r:id="rId61" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000308"/>
-    <hyperlink ref="B29" r:id="rId62" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000055"/>
-    <hyperlink ref="B22" r:id="rId63" location="has_information_entity_component"/>
-    <hyperlink ref="B23" r:id="rId64" location="componet_of_information_entity"/>
+    <hyperlink ref="A17" r:id="rId35" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23ZeroDimensionalRegion"/>
+    <hyperlink ref="B17" r:id="rId36" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000018"/>
+    <hyperlink ref="A18" r:id="rId37" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23OneDimensionalRegion"/>
+    <hyperlink ref="B18" r:id="rId38" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000026"/>
+    <hyperlink ref="A19" r:id="rId39" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23TwoDimensionalRegion"/>
+    <hyperlink ref="B19" r:id="rId40" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000009"/>
+    <hyperlink ref="A20" r:id="rId41" display="//www.google.com/url?q=http%3A%2F%2Fwww.ifomis.org%2Fbfo%2F1.1%2Fsnap%23ThreeDimensionalRegion"/>
+    <hyperlink ref="B20" r:id="rId42" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000028"/>
+    <hyperlink ref="A21" r:id="rId43" display="//www.google.com/url?q=http%3A%2F%2Fpurl.org%2Fobo%2Fowl%2FOBO_REL%23bearer_of"/>
+    <hyperlink ref="B21" r:id="rId44" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000053"/>
+    <hyperlink ref="A22" r:id="rId45" display="//www.google.com/url?q=http%3A%2F%2Fpurl.org%2Fobo%2Fowl%2FOBO_REL%23inheres_in"/>
+    <hyperlink ref="B22" r:id="rId46" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000052"/>
+    <hyperlink ref="A23" r:id="rId47" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_part"/>
+    <hyperlink ref="G23" r:id="rId48" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000051"/>
+    <hyperlink ref="A24" r:id="rId49" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23part_of"/>
+    <hyperlink ref="G24" r:id="rId50" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000050"/>
+    <hyperlink ref="A25" r:id="rId51" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_participant"/>
+    <hyperlink ref="B25" r:id="rId52" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000057"/>
+    <hyperlink ref="A26" r:id="rId53" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23participates_in"/>
+    <hyperlink ref="B26" r:id="rId54" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000056"/>
+    <hyperlink ref="A27" r:id="rId55" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000294"/>
+    <hyperlink ref="B27" r:id="rId56" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000059"/>
+    <hyperlink ref="A28" r:id="rId57" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000297"/>
+    <hyperlink ref="B28" r:id="rId58" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000058"/>
+    <hyperlink ref="A29" r:id="rId59" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000300"/>
+    <hyperlink ref="B29" r:id="rId60" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000054"/>
+    <hyperlink ref="A30" r:id="rId61" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000308"/>
+    <hyperlink ref="B30" r:id="rId62" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000055"/>
+    <hyperlink ref="B23" r:id="rId63" location="has_information_entity_component"/>
+    <hyperlink ref="B24" r:id="rId64" location="componet_of_information_entity"/>
+    <hyperlink ref="A16" r:id="rId65" location="Process"/>
+    <hyperlink ref="B16" r:id="rId66"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId65"/>
+  <pageSetup orientation="portrait" r:id="rId67"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correct typo: componet_of_information_entity -> component_of_information_entity
</commit_message>
<xml_diff>
--- a/branches/2014-06-13/doc/termsMapping.xlsx
+++ b/branches/2014-06-13/doc/termsMapping.xlsx
@@ -343,10 +343,10 @@
     <t>http://purl.obolibrary.org/obo/iao/dev/iao-main.owl#has_information_entity_component</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/iao/dev/iao-main.owl#componet_of_information_entity</t>
-  </si>
-  <si>
     <t>http://www.ifomis.org/bfo/1.1/span#Process</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/iao/dev/iao-main.owl#component_of_information_entity</t>
   </si>
 </sst>
 </file>
@@ -781,7 +781,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>58</v>
@@ -1208,7 +1208,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>94</v>
@@ -1450,7 +1450,7 @@
     <hyperlink ref="A30" r:id="rId61" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000308"/>
     <hyperlink ref="B30" r:id="rId62" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000055"/>
     <hyperlink ref="B23" r:id="rId63" location="has_information_entity_component"/>
-    <hyperlink ref="B24" r:id="rId64" location="componet_of_information_entity"/>
+    <hyperlink ref="B24" r:id="rId64" location="component_of_information_entity"/>
     <hyperlink ref="A16" r:id="rId65" location="Process"/>
     <hyperlink ref="B16" r:id="rId66"/>
   </hyperlinks>

</xml_diff>

<commit_message>
updated IRIs of two newly-added IAO relations
</commit_message>
<xml_diff>
--- a/branches/2014-06-13/doc/termsMapping.xlsx
+++ b/branches/2014-06-13/doc/termsMapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>http://purl.org/obo/owl/OBO_REL#bearer_of</t>
   </si>
@@ -67,12 +67,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000003</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/BFO_0000051</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/BFO_0000050</t>
-  </si>
-  <si>
     <t>http://www.obofoundry.org/ro/ro.owl#participates_in</t>
   </si>
   <si>
@@ -268,9 +262,6 @@
     <t>BFO 2.0 Labels</t>
   </si>
   <si>
-    <t>has part</t>
-  </si>
-  <si>
     <t>not used in IAO, but used to define 'bearer of'</t>
   </si>
   <si>
@@ -283,9 +274,6 @@
     <t>OBI terms: is_concretized_as, term deprecated in OBI</t>
   </si>
   <si>
-    <t>part of</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -340,13 +328,13 @@
     <t>not use RO 'part of', BFO domain but RO term, IRI created in BFO pre-Graz</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/iao/dev/iao-main.owl#has_information_entity_component</t>
-  </si>
-  <si>
     <t>http://www.ifomis.org/bfo/1.1/span#Process</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/iao/dev/iao-main.owl#component_of_information_entity</t>
+    <t>http://purl.obolibrary.org/obo/IAO_0000708</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IAO_0000709</t>
   </si>
 </sst>
 </file>
@@ -396,7 +384,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,12 +394,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE599"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,13 +451,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -780,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,553 +777,515 @@
     <col min="7" max="7" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+      <c r="G1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="E22" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>106</v>
+        <v>90</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>107</v>
+        <v>90</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>103</v>
+        <v>90</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>105</v>
+        <v>90</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>25</v>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="B30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="9" t="s">
+      <c r="C30" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>86</v>
+      <c r="E30" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -1363,26 +1307,26 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1434,27 +1378,25 @@
     <hyperlink ref="A22" r:id="rId45" display="//www.google.com/url?q=http%3A%2F%2Fpurl.org%2Fobo%2Fowl%2FOBO_REL%23inheres_in"/>
     <hyperlink ref="B22" r:id="rId46" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000052"/>
     <hyperlink ref="A23" r:id="rId47" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_part"/>
-    <hyperlink ref="G23" r:id="rId48" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000051"/>
-    <hyperlink ref="A24" r:id="rId49" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23part_of"/>
-    <hyperlink ref="G24" r:id="rId50" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000050"/>
-    <hyperlink ref="A25" r:id="rId51" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_participant"/>
-    <hyperlink ref="B25" r:id="rId52" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000057"/>
-    <hyperlink ref="A26" r:id="rId53" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23participates_in"/>
-    <hyperlink ref="B26" r:id="rId54" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000056"/>
-    <hyperlink ref="A27" r:id="rId55" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000294"/>
-    <hyperlink ref="B27" r:id="rId56" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000059"/>
-    <hyperlink ref="A28" r:id="rId57" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000297"/>
-    <hyperlink ref="B28" r:id="rId58" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000058"/>
-    <hyperlink ref="A29" r:id="rId59" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000300"/>
-    <hyperlink ref="B29" r:id="rId60" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000054"/>
-    <hyperlink ref="A30" r:id="rId61" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000308"/>
-    <hyperlink ref="B30" r:id="rId62" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000055"/>
-    <hyperlink ref="B23" r:id="rId63" location="has_information_entity_component"/>
-    <hyperlink ref="B24" r:id="rId64" location="component_of_information_entity"/>
-    <hyperlink ref="A16" r:id="rId65" location="Process"/>
-    <hyperlink ref="B16" r:id="rId66"/>
+    <hyperlink ref="A24" r:id="rId48" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23part_of"/>
+    <hyperlink ref="A25" r:id="rId49" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23has_participant"/>
+    <hyperlink ref="B25" r:id="rId50" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000057"/>
+    <hyperlink ref="A26" r:id="rId51" display="//www.google.com/url?q=http%3A%2F%2Fwww.obofoundry.org%2Fro%2Fro.owl%23participates_in"/>
+    <hyperlink ref="B26" r:id="rId52" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000056"/>
+    <hyperlink ref="A27" r:id="rId53" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000294"/>
+    <hyperlink ref="B27" r:id="rId54" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000059"/>
+    <hyperlink ref="A28" r:id="rId55" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000297"/>
+    <hyperlink ref="B28" r:id="rId56" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000058"/>
+    <hyperlink ref="A29" r:id="rId57" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000300"/>
+    <hyperlink ref="B29" r:id="rId58" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000054"/>
+    <hyperlink ref="A30" r:id="rId59" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000308"/>
+    <hyperlink ref="B30" r:id="rId60" display="//www.google.com/url?q=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FBFO_0000055"/>
+    <hyperlink ref="A16" r:id="rId61" location="Process"/>
+    <hyperlink ref="B16" r:id="rId62"/>
+    <hyperlink ref="B24" r:id="rId63"/>
+    <hyperlink ref="B23" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId67"/>
+  <pageSetup orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
</xml_diff>